<commit_message>
fix endianess issue in peerings, the content in the EEPROM is always BigEndian format
</commit_message>
<xml_diff>
--- a/Documentation/EEPROM_Layout.xlsx
+++ b/Documentation/EEPROM_Layout.xlsx
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,7 +1133,7 @@
         <v>97</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="C36" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
add generic commands to HBWChannel,; fix using peering parameters for TOGGLE and BLINK_TOGGLE
</commit_message>
<xml_diff>
--- a/Documentation/EEPROM_Layout.xlsx
+++ b/Documentation/EEPROM_Layout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="132">
   <si>
     <t>Adresse start</t>
   </si>
@@ -45,9 +45,6 @@
     <t>0x0005</t>
   </si>
   <si>
-    <t>0x0006</t>
-  </si>
-  <si>
     <t>0x0007</t>
   </si>
   <si>
@@ -288,9 +285,6 @@
     <t>Dimmer-Peering 2 bis 30</t>
   </si>
   <si>
-    <t>0x02D4</t>
-  </si>
-  <si>
     <t>0x0032</t>
   </si>
   <si>
@@ -345,9 +339,6 @@
     <t>0x00FA:2</t>
   </si>
   <si>
-    <t>0x00FA:4</t>
-  </si>
-  <si>
     <t>0x00FB</t>
   </si>
   <si>
@@ -369,17 +360,65 @@
     <t>0x00FA:3</t>
   </si>
   <si>
-    <t>0x00FA:1</t>
-  </si>
-  <si>
     <t>0x00F7</t>
+  </si>
+  <si>
+    <t>0x02E4</t>
+  </si>
+  <si>
+    <t>0x0006:0</t>
+  </si>
+  <si>
+    <t>0x0006:1</t>
+  </si>
+  <si>
+    <t>LED_FEEDBACK</t>
+  </si>
+  <si>
+    <t>0x0008:0</t>
+  </si>
+  <si>
+    <t>0x0008:1</t>
+  </si>
+  <si>
+    <t>INPUT_LOCKED</t>
+  </si>
+  <si>
+    <t>0x0008:2</t>
+  </si>
+  <si>
+    <t>0x0008:7</t>
+  </si>
+  <si>
+    <t>0x00FA:5</t>
+  </si>
+  <si>
+    <t>0x00FA:6</t>
+  </si>
+  <si>
+    <t>BLINK_ON_TIME</t>
+  </si>
+  <si>
+    <t>0x0100</t>
+  </si>
+  <si>
+    <t>BLINK_OFF_TIME</t>
+  </si>
+  <si>
+    <t>0x0101</t>
+  </si>
+  <si>
+    <t>BLINK_QUANTITY</t>
+  </si>
+  <si>
+    <t>0x0102</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,7 +466,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -485,7 +524,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -517,10 +556,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -552,7 +590,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -728,14 +765,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
@@ -743,7 +780,7 @@
     <col min="4" max="4" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -751,10 +788,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -765,7 +802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -776,7 +813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -787,565 +824,631 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" t="s">
+    <row r="27" spans="1:3">
+      <c r="A27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="28" spans="1:3">
+      <c r="A28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C24" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="29" spans="1:3">
+      <c r="A29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" t="s">
         <v>94</v>
       </c>
-      <c r="C29" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" t="s">
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C33" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C35" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:3">
+      <c r="A36" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="C39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C36" t="s">
+      <c r="B43" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C45" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C37" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C38" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C39" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C40" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C41" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C42" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+    <row r="48" spans="1:3">
+      <c r="A48" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="B48" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C44" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C45" t="s">
+    <row r="49" spans="1:3">
+      <c r="A49" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C49" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C46" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C47" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C48" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C49" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" s="2" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>112</v>
       </c>
       <c r="C50" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C51" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B52" s="2" t="s">
+    <row r="55" spans="1:3">
+      <c r="A55" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C56" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C59" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C60" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C53" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B54" s="3" t="s">
+    <row r="61" spans="1:3">
+      <c r="A61" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C54" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="B61" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C55" t="s">
-        <v>65</v>
+      <c r="C61" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1355,24 +1458,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>